<commit_message>
TL a bunch (see git commit) and fix <pause> breaking options loading
</commit_message>
<xml_diff>
--- a/tl/P11210.MES.BIN.xlsx
+++ b/tl/P11210.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C811570C-9D54-4AF0-A8E0-0585D9FFA4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EEEBB3-63C8-4626-9938-5AD0969220EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="4290" windowWidth="55245" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P11210.MES.BIN" sheetId="1" r:id="rId1"/>

</xml_diff>